<commit_message>
added table to document
</commit_message>
<xml_diff>
--- a/Insert_Text_Into_Cell_In_SpreadSheet_In_Excel/Excel_Folder/sample.xlsx
+++ b/Insert_Text_Into_Cell_In_SpreadSheet_In_Excel/Excel_Folder/sample.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <x:workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bdas\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{DAD0FEB2-4265-40D7-B875-8A75E7EDDBCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F371911E-93D7-43F8-BD57-4C414028DFAB}"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <x:bookViews>
+    <x:workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F371911E-93D7-43F8-BD57-4C414028DFAB}"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <x:sheet name="Sheet2" sheetId="2" r:id="R59e06f8eafc640ec"/>
+  </x:sheets>
+  <x:calcPr calcId="191029"/>
+  <x:extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+    </x:ext>
+    <x:ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
@@ -30,9 +31,17 @@
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
-</workbook>
+    </x:ext>
+  </x:extLst>
+</x:workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:si>
+    <x:t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -410,4 +419,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetData>
+    <x:row r="2">
+      <x:c r="B2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+</x:worksheet>
 </file>
</xml_diff>